<commit_message>
Solution for q7.09 and partial solution to q7.05
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="q7-02" sheetId="5" r:id="rId4"/>
     <sheet name="q7-03" sheetId="6" r:id="rId5"/>
     <sheet name="q7-04" sheetId="7" r:id="rId6"/>
+    <sheet name="q7-09" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="49">
   <si>
     <t>l</t>
   </si>
@@ -147,6 +148,30 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>1/10</t>
+  </si>
+  <si>
+    <t>2/9</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>3/6</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>7/8</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -975,7 +1000,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1049,6 +1074,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,14 +1104,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -25316,6 +25356,811 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>62246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62245</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>10500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Conector reto 68"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="61" idx="2"/>
+          <a:endCxn id="31" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="390524" y="3024521"/>
+          <a:ext cx="814721" cy="1662754"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -37412"/>
+            <a:gd name="adj2" fmla="val 112909"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>316804</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector reto 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="31" idx="2"/>
+          <a:endCxn id="33" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="697804" y="3151800"/>
+          <a:ext cx="454721" cy="636671"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>21000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Conector reto 61"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="33" idx="4"/>
+          <a:endCxn id="61" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="570525" y="4095750"/>
+          <a:ext cx="0" cy="411525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>62246</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector reto 13"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="31" idx="6"/>
+          <a:endCxn id="32" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1512525" y="3151800"/>
+          <a:ext cx="454721" cy="636671"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Conector reto 14"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="4"/>
+          <a:endCxn id="31" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1332525" y="2560275"/>
+          <a:ext cx="0" cy="411525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Fluxograma: Conector 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="2200275"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector reto 21"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="6"/>
+          <a:endCxn id="32" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1512525" y="2380275"/>
+          <a:ext cx="582000" cy="1355475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Fluxograma: Conector 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="2971800"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>z</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Fluxograma: Conector 31"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914525" y="3735750"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>w</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Fluxograma: Conector 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="3735750"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>y</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>21000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Fluxograma: Conector 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="4507275"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>x</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>128254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>62246</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>10500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Conector reto 64"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="3"/>
+          <a:endCxn id="61" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="750525" y="4043029"/>
+          <a:ext cx="1216721" cy="644246"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -25634,7 +26479,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="47">
+      <c r="B3" s="54">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -25675,7 +26520,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="48"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -25712,7 +26557,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="48"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -25747,7 +26592,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -25780,7 +26625,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -25811,7 +26656,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="47">
+      <c r="B8" s="54">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -25842,7 +26687,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="48"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -25860,7 +26705,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -25881,7 +26726,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="48"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -25917,7 +26762,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="48"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -25956,7 +26801,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="48"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -25993,7 +26838,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="48"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -26028,7 +26873,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="49"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -26061,7 +26906,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="47">
+      <c r="B16" s="54">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -26094,7 +26939,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="48"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -26123,7 +26968,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="48"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -26141,7 +26986,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -26159,7 +27004,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="48"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -26177,7 +27022,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="48"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -26195,7 +27040,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="48"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -26213,7 +27058,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="48"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -26231,7 +27076,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -26249,7 +27094,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="47">
+      <c r="B25" s="54">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -26269,7 +27114,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="48"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -26287,7 +27132,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="48"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -26305,7 +27150,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="48"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -26323,7 +27168,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="48"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -26341,7 +27186,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="48"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -26359,7 +27204,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="48"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -26377,7 +27222,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="49"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -26395,7 +27240,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="47">
+      <c r="B33" s="54">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -26415,7 +27260,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="48"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -26433,7 +27278,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -26451,7 +27296,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="48"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -26469,7 +27314,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="49"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -26660,8 +27505,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -26733,8 +27578,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -26751,8 +27596,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -26827,8 +27672,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -26851,8 +27696,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -26927,8 +27772,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -26951,8 +27796,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -27024,8 +27869,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -27048,8 +27893,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -27121,8 +27966,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -27145,8 +27990,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -27218,8 +28063,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="50"/>
-      <c r="I59" s="50"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="57"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -27279,10 +28124,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="51"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -27367,10 +28212,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="51" t="s">
+      <c r="H9" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="51"/>
+      <c r="I9" s="58"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -27388,10 +28233,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="51"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -27482,10 +28327,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="51" t="s">
+      <c r="H19" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="51"/>
+      <c r="I19" s="58"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -27509,10 +28354,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="51" t="s">
+      <c r="H22" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="51"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -27603,10 +28448,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="51" t="s">
+      <c r="H29" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="51"/>
+      <c r="I29" s="58"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -27630,10 +28475,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="51" t="s">
+      <c r="H32" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="51"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -27721,10 +28566,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="51" t="s">
+      <c r="H39" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="51"/>
+      <c r="I39" s="58"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -27768,10 +28613,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="51" t="s">
+      <c r="H42" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="51"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -27856,10 +28701,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="51" t="s">
+      <c r="H49" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="51"/>
+      <c r="I49" s="58"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -27903,10 +28748,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="51" t="s">
+      <c r="H52" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="51"/>
+      <c r="I52" s="58"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -27991,10 +28836,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="51" t="s">
+      <c r="H59" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="51"/>
+      <c r="I59" s="58"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -28038,10 +28883,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="51" t="s">
+      <c r="H62" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="51"/>
+      <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -28126,10 +28971,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="51" t="s">
+      <c r="H69" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="51"/>
+      <c r="I69" s="58"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -28173,10 +29018,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="51" t="s">
+      <c r="H72" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="51"/>
+      <c r="I72" s="58"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -28261,10 +29106,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="51" t="s">
+      <c r="H79" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="51"/>
+      <c r="I79" s="58"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -28308,10 +29153,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="51" t="s">
+      <c r="H82" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="51"/>
+      <c r="I82" s="58"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -28396,14 +29241,1205 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="51" t="s">
+      <c r="H89" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="51"/>
+      <c r="I89" s="58"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
       <c r="L89" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="M89" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H82:I82"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AC89"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="AC75" sqref="AC75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="25" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="58"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K3" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="58"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K13" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R15" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K16" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16" s="41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B19" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="58"/>
+      <c r="K19" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AC21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B22" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="58"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="K23" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N25" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P25" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S25" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="K26" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P26" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="R26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S26" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B29" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="58"/>
+      <c r="K29" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B32" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="58"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K33" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P35" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q35" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R35" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S35" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K36" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M36" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O36" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P36" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q36" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R36" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S36" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="58"/>
+      <c r="K39" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L39" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="58"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K43" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M45" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N45" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O45" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P45" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q45" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R45" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S45" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K46" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M46" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="N46" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O46" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P46" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q46" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R46" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S46" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B49" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="58"/>
+      <c r="K49" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B52" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="58"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K53" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K55" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L55" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M55" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N55" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O55" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P55" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q55" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R55" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S55" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K56" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O56" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P56" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q56" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R56" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S56" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B59" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I59" s="58"/>
+      <c r="K59" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L59" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M59" s="39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="58"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K63" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L63" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K65" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L65" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M65" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N65" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O65" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P65" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q65" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R65" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S65" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K66" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="M66" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N66" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O66" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P66" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q66" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R66" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S66" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="58"/>
+      <c r="K69" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L69" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M69" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I72" s="58"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K73" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K75" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L75" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M75" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N75" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O75" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P75" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q75" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R75" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S75" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K76" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L76" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M76" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N76" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O76" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P76" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q76" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R76" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S76" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B79" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="1"/>
+      <c r="H79" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I79" s="58"/>
+      <c r="K79" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L79" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M79" s="39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B82" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" s="1"/>
+      <c r="H82" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I82" s="58"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K83" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L83" s="42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="K85" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L85" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N85" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O85" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="P85" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q85" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="R85" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S85" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K86" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L86" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="M86" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O86" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P86" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q86" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="R86" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="S86" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B89" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="1"/>
+      <c r="H89" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I89" s="58"/>
+      <c r="K89" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L89" s="37" t="s">
         <v>28</v>
       </c>
       <c r="M89" s="39" t="s">
@@ -28437,1202 +30473,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC89"/>
-  <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="AC75" sqref="AC75"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="25" width="3.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="51"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K3" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K6" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="51"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="39"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="51"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K13" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O15" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P15" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q15" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R15" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S15" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K16" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="R16" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="51"/>
-      <c r="K19" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="AC21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="51"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="K23" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="N23" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L25" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M25" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N25" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O25" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P25" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q25" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R25" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S25" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="K26" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N26" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="R26" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S26" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="51"/>
-      <c r="K29" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="51"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K33" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L33" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="M33" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="K35" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L35" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M35" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N35" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O35" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P35" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q35" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R35" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S35" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K36" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L36" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N36" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O36" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P36" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q36" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R36" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S36" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="51"/>
-      <c r="K39" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I42" s="51"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K43" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L43" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="K45" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L45" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M45" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N45" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O45" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P45" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q45" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R45" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S45" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K46" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L46" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M46" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="N46" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O46" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P46" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q46" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R46" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S46" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B49" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="51"/>
-      <c r="K49" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L49" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M49" s="39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="D52" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I52" s="51"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K53" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L53" s="33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="K55" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L55" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M55" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N55" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O55" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P55" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q55" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R55" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S55" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K56" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L56" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="N56" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O56" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P56" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q56" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R56" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S56" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B59" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E59" s="1"/>
-      <c r="F59" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I59" s="51"/>
-      <c r="K59" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L59" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M59" s="39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B62" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I62" s="51"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K63" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L63" s="33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="K65" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L65" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M65" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N65" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O65" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P65" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q65" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R65" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S65" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K66" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L66" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="M66" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N66" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O66" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P66" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q66" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R66" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S66" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G69" s="1"/>
-      <c r="H69" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I69" s="51"/>
-      <c r="K69" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L69" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M69" s="39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B72" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E72" s="1"/>
-      <c r="F72" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I72" s="51"/>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K73" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L73" s="33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="K75" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L75" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M75" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N75" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O75" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P75" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q75" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R75" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S75" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K76" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L76" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="M76" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N76" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O76" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P76" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q76" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R76" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S76" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B79" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E79" s="1"/>
-      <c r="F79" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="1"/>
-      <c r="H79" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I79" s="51"/>
-      <c r="K79" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L79" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M79" s="39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B82" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E82" s="1"/>
-      <c r="F82" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G82" s="1"/>
-      <c r="H82" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="I82" s="51"/>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K83" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L83" s="42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="K85" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="L85" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M85" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N85" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="O85" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="P85" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q85" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="R85" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="S85" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K86" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L86" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="M86" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N86" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O86" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="P86" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q86" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="R86" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="S86" s="33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B89" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C89" s="1"/>
-      <c r="D89" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="E89" s="1"/>
-      <c r="F89" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G89" s="1"/>
-      <c r="H89" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="I89" s="51"/>
-      <c r="K89" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L89" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M89" s="39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H82:I82"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
@@ -29650,54 +30495,54 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K3" s="52"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="46"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K6" s="55"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
     </row>
     <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -29707,8 +30552,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -29724,8 +30569,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -29761,7 +30606,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="53" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="33" t="s">
@@ -29806,8 +30651,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -29823,8 +30668,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -29857,7 +30702,7 @@
       <c r="B24" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="56" t="s">
+      <c r="K24" s="53" t="s">
         <v>10</v>
       </c>
       <c r="L24" s="33" t="s">
@@ -29903,8 +30748,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -29922,4 +30767,108 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="48"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="48"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="38"/>
+      <c r="L4" s="53"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="48"/>
+      <c r="L8" s="53"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="38"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="48"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding solution for q7-10
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="q7-06" sheetId="9" r:id="rId7"/>
     <sheet name="q7-08" sheetId="10" r:id="rId8"/>
     <sheet name="q7-09" sheetId="8" r:id="rId9"/>
+    <sheet name="q7-10" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="83">
   <si>
     <t>l</t>
   </si>
@@ -270,6 +271,12 @@
   </si>
   <si>
     <t>17/20</t>
+  </si>
+  <si>
+    <t>1/6</t>
+  </si>
+  <si>
+    <t>2/3</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1105,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1210,6 +1217,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -40575,6 +40585,422 @@
         <a:ln>
           <a:tailEnd type="stealth"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>136804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>71771</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector reto 7"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="3"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="570525" y="1279804"/>
+          <a:ext cx="263246" cy="454721"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>379050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Fluxograma: Conector 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="972525"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Fluxograma: Conector 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="1734525"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>u</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>379050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Fluxograma: Conector 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="1734525"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>v</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>62247</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>72746</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector reto 26"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="1"/>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="294788" y="1300984"/>
+          <a:ext cx="634721" cy="337804"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>326329</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>136804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>199050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector reto 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="5"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1088329" y="1279804"/>
+          <a:ext cx="253721" cy="454721"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -40914,7 +41340,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="63">
+      <c r="B3" s="64">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -40955,7 +41381,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="64"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -40992,7 +41418,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="64"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -41027,7 +41453,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -41060,7 +41486,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="65"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -41091,7 +41517,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="63">
+      <c r="B8" s="64">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -41122,7 +41548,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="64"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -41140,7 +41566,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="64"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -41161,7 +41587,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="64"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -41197,7 +41623,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="64"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -41236,7 +41662,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="64"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -41273,7 +41699,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="64"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -41308,7 +41734,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="65"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -41341,7 +41767,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="63">
+      <c r="B16" s="64">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -41374,7 +41800,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -41403,7 +41829,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="64"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -41421,7 +41847,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="64"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -41439,7 +41865,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="64"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -41457,7 +41883,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="64"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -41475,7 +41901,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="64"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -41493,7 +41919,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="64"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -41511,7 +41937,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="65"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -41529,7 +41955,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="63">
+      <c r="B25" s="64">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -41549,7 +41975,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="64"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -41567,7 +41993,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="64"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -41585,7 +42011,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="64"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -41603,7 +42029,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="64"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -41621,7 +42047,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="64"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -41639,7 +42065,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="64"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -41657,7 +42083,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="65"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -41675,7 +42101,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="63">
+      <c r="B33" s="64">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -41695,7 +42121,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="64"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -41713,7 +42139,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="64"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -41731,7 +42157,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="64"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -41749,7 +42175,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="65"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -41776,6 +42202,63 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="44" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="63"/>
+      <c r="C1" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="63"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="1"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="38"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -41940,8 +42423,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -42013,8 +42496,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -42031,8 +42514,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -42107,8 +42590,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -42131,8 +42614,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -42207,8 +42690,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -42231,8 +42714,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -42304,8 +42787,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -42328,8 +42811,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="66"/>
-      <c r="I42" s="66"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -42401,8 +42884,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="66"/>
-      <c r="I49" s="66"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -42425,8 +42908,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -42498,8 +42981,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
+      <c r="H59" s="67"/>
+      <c r="I59" s="67"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -42559,10 +43042,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -42647,10 +43130,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="68"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -42668,10 +43151,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="67"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -42762,10 +43245,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="67" t="s">
+      <c r="H19" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="68"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -42789,10 +43272,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="67" t="s">
+      <c r="H22" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="67"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -42883,10 +43366,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="67" t="s">
+      <c r="H29" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="67"/>
+      <c r="I29" s="68"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -42910,10 +43393,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="67" t="s">
+      <c r="H32" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="67"/>
+      <c r="I32" s="68"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -43001,10 +43484,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="67" t="s">
+      <c r="H39" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="67"/>
+      <c r="I39" s="68"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -43048,10 +43531,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="67" t="s">
+      <c r="H42" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="67"/>
+      <c r="I42" s="68"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -43136,10 +43619,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="67" t="s">
+      <c r="H49" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="67"/>
+      <c r="I49" s="68"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -43183,10 +43666,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="67" t="s">
+      <c r="H52" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="67"/>
+      <c r="I52" s="68"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -43271,10 +43754,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="67" t="s">
+      <c r="H59" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="67"/>
+      <c r="I59" s="68"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -43318,10 +43801,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="67" t="s">
+      <c r="H62" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="67"/>
+      <c r="I62" s="68"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -43406,10 +43889,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="67" t="s">
+      <c r="H69" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="67"/>
+      <c r="I69" s="68"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -43453,10 +43936,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="67" t="s">
+      <c r="H72" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="67"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -43541,10 +44024,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="67" t="s">
+      <c r="H79" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="67"/>
+      <c r="I79" s="68"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -43588,10 +44071,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="67" t="s">
+      <c r="H82" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="67"/>
+      <c r="I82" s="68"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -43676,10 +44159,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="67" t="s">
+      <c r="H89" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="67"/>
+      <c r="I89" s="68"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -43692,12 +44175,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -43710,6 +44187,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43745,10 +44228,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -43833,10 +44316,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="68"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -43854,10 +44337,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="67"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -43948,10 +44431,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="67" t="s">
+      <c r="H19" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="68"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -43980,10 +44463,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="67" t="s">
+      <c r="H22" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="67"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -44074,10 +44557,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="67" t="s">
+      <c r="H29" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="67"/>
+      <c r="I29" s="68"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -44101,10 +44584,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="67" t="s">
+      <c r="H32" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="67"/>
+      <c r="I32" s="68"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -44192,10 +44675,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="67" t="s">
+      <c r="H39" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="67"/>
+      <c r="I39" s="68"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -44239,10 +44722,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="67" t="s">
+      <c r="H42" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="67"/>
+      <c r="I42" s="68"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -44327,10 +44810,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="67" t="s">
+      <c r="H49" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="67"/>
+      <c r="I49" s="68"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -44374,10 +44857,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="67" t="s">
+      <c r="H52" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="67"/>
+      <c r="I52" s="68"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -44462,10 +44945,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="67" t="s">
+      <c r="H59" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="67"/>
+      <c r="I59" s="68"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -44509,10 +44992,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="67" t="s">
+      <c r="H62" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="67"/>
+      <c r="I62" s="68"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -44597,10 +45080,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="67" t="s">
+      <c r="H69" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="67"/>
+      <c r="I69" s="68"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -44644,10 +45127,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="67" t="s">
+      <c r="H72" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="67"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -44732,10 +45215,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="67" t="s">
+      <c r="H79" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="67"/>
+      <c r="I79" s="68"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -44779,10 +45262,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="67" t="s">
+      <c r="H82" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="67"/>
+      <c r="I82" s="68"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -44867,10 +45350,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="67" t="s">
+      <c r="H89" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="67"/>
+      <c r="I89" s="68"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -44883,6 +45366,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -44895,12 +45384,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44930,8 +45413,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -44987,8 +45470,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -45004,8 +45487,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -45086,8 +45569,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -45103,8 +45586,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -45183,8 +45666,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -45230,8 +45713,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -46282,7 +46765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="Y56" sqref="Y56"/>
     </sheetView>
   </sheetViews>
@@ -46886,8 +47369,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -46941,8 +47424,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>

<commit_message>
Adding solution for q7-11
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="86">
   <si>
     <t>l</t>
   </si>
@@ -273,10 +273,19 @@
     <t>17/20</t>
   </si>
   <si>
-    <t>1/6</t>
+    <t>2/3</t>
   </si>
   <si>
-    <t>2/3</t>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>1/4</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
+    <t>3/4</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1217,6 +1226,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -40610,44 +40622,98 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12993</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>135648</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>162705</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Elipse 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19544282">
+          <a:off x="1384593" y="44568"/>
+          <a:ext cx="884655" cy="1832637"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>189525</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>136804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>71771</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>20025</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="8" name="Conector reto 7"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="13" idx="0"/>
+          <a:stCxn id="13" idx="0"/>
+          <a:endCxn id="10" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="570525" y="1279804"/>
+        <a:xfrm flipV="1">
+          <a:off x="570525" y="517804"/>
           <a:ext cx="263246" cy="454721"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:prstDash val="dash"/>
           <a:tailEnd type="stealth"/>
         </a:ln>
-        <a:effectLst>
-          <a:glow rad="63500">
-            <a:schemeClr val="bg2">
-              <a:lumMod val="25000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:glow>
-        </a:effectLst>
+        <a:effectLst/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -40668,15 +40734,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>20025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>379050</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>189525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -40749,15 +40815,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>20025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>369525</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>189525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -40830,15 +40896,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>20025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>379050</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>189525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -40911,32 +40977,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>62247</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>72746</xdr:rowOff>
+      <xdr:colOff>316804</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>136805</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="20" name="Conector reto 26"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="13" idx="1"/>
-          <a:endCxn id="10" idx="2"/>
+          <a:stCxn id="13" idx="5"/>
+          <a:endCxn id="13" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="294788" y="1300984"/>
-          <a:ext cx="634721" cy="337804"/>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="1090125" y="1253026"/>
+          <a:ext cx="127279" cy="307279"/>
         </a:xfrm>
-        <a:prstGeom prst="curvedConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -221027"/>
+            <a:gd name="adj2" fmla="val 174395"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:prstDash val="dash"/>
@@ -40963,15 +41032,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>326329</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>136804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>199050</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>20025</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -41017,6 +41086,642 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Fluxograma: Conector 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="1905000"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Fluxograma: Conector 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="1905000"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>u</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Fluxograma: Conector 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2667000" y="1905000"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>v</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector reto 26"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="6"/>
+          <a:endCxn id="25" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="741000" y="2085000"/>
+          <a:ext cx="783000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector reto 28"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="25" idx="6"/>
+          <a:endCxn id="26" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1884000" y="2085000"/>
+          <a:ext cx="783000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>360000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Conector reto 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="741000" y="2085000"/>
+          <a:ext cx="783000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="stealth"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>440331</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>34387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>159289</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>157042</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Elipse 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17762800">
+          <a:off x="543282" y="883936"/>
+          <a:ext cx="884655" cy="1090558"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>87910</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>158211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238129</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Elipse 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="1942338" y="2151883"/>
+          <a:ext cx="708564" cy="912219"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>97435</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247654</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Elipse 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3094863" y="2180458"/>
+          <a:ext cx="708564" cy="912219"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>87910</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238129</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Elipse 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="799338" y="2180458"/>
+          <a:ext cx="708564" cy="912219"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -41340,7 +42045,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="64">
+      <c r="B3" s="65">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -41381,7 +42086,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="65"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -41418,7 +42123,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -41453,7 +42158,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -41486,7 +42191,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -41517,7 +42222,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="64">
+      <c r="B8" s="65">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -41548,7 +42253,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -41566,7 +42271,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="65"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -41587,7 +42292,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -41623,7 +42328,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -41662,7 +42367,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="65"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -41699,7 +42404,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="65"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -41734,7 +42439,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="66"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -41767,7 +42472,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="64">
+      <c r="B16" s="65">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -41800,7 +42505,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="65"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -41829,7 +42534,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="65"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -41847,7 +42552,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="65"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -41865,7 +42570,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="65"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -41883,7 +42588,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="65"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -41901,7 +42606,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="65"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -41919,7 +42624,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="65"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -41937,7 +42642,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="66"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -41955,7 +42660,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="64">
+      <c r="B25" s="65">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -41975,7 +42680,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="65"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -41993,7 +42698,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="65"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -42011,7 +42716,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="65"/>
+      <c r="B28" s="66"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -42029,7 +42734,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="65"/>
+      <c r="B29" s="66"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -42047,7 +42752,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="65"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -42065,7 +42770,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="65"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -42083,7 +42788,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="66"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -42101,7 +42806,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="64">
+      <c r="B33" s="65">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -42121,7 +42826,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="65"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -42139,7 +42844,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="65"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -42157,7 +42862,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="65"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -42175,7 +42880,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="66"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -42207,52 +42912,78 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="44" width="5.7109375" customWidth="1"/>
+    <col min="2" max="45" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="63"/>
-      <c r="C1" s="56" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="63"/>
+      <c r="D2" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="56"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="63"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="57"/>
+      <c r="C3" s="1"/>
+      <c r="H3" s="58"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="38"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="63"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="1"/>
-      <c r="G2" s="58"/>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="1"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="56" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>45</v>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -42423,8 +43154,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -42496,8 +43227,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -42514,8 +43245,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -42590,8 +43321,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -42614,8 +43345,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -42690,8 +43421,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -42714,8 +43445,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -42787,8 +43518,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -42811,8 +43542,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="68"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -42884,8 +43615,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="67"/>
-      <c r="I49" s="67"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="68"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -42908,8 +43639,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="68"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -42981,8 +43712,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="67"/>
-      <c r="I59" s="67"/>
+      <c r="H59" s="68"/>
+      <c r="I59" s="68"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -43042,10 +43773,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="68"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -43130,10 +43861,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -43151,10 +43882,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="68"/>
+      <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -43245,10 +43976,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="68" t="s">
+      <c r="H19" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="68"/>
+      <c r="I19" s="69"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -43272,10 +44003,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="68" t="s">
+      <c r="H22" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="68"/>
+      <c r="I22" s="69"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -43366,10 +44097,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="68" t="s">
+      <c r="H29" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="68"/>
+      <c r="I29" s="69"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -43393,10 +44124,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="68" t="s">
+      <c r="H32" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="68"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -43484,10 +44215,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="68" t="s">
+      <c r="H39" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="68"/>
+      <c r="I39" s="69"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -43531,10 +44262,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="68" t="s">
+      <c r="H42" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="68"/>
+      <c r="I42" s="69"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -43619,10 +44350,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="68" t="s">
+      <c r="H49" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="68"/>
+      <c r="I49" s="69"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -43666,10 +44397,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="68" t="s">
+      <c r="H52" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="68"/>
+      <c r="I52" s="69"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -43754,10 +44485,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="68" t="s">
+      <c r="H59" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="68"/>
+      <c r="I59" s="69"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -43801,10 +44532,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="68" t="s">
+      <c r="H62" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="68"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -43889,10 +44620,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="68" t="s">
+      <c r="H69" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="68"/>
+      <c r="I69" s="69"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -43936,10 +44667,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="68" t="s">
+      <c r="H72" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="68"/>
+      <c r="I72" s="69"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -44024,10 +44755,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="68" t="s">
+      <c r="H79" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="68"/>
+      <c r="I79" s="69"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -44071,10 +44802,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="68" t="s">
+      <c r="H82" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="68"/>
+      <c r="I82" s="69"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -44159,10 +44890,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="68" t="s">
+      <c r="H89" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="68"/>
+      <c r="I89" s="69"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -44175,6 +44906,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -44187,12 +44924,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44228,10 +44959,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="68"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -44316,10 +45047,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -44337,10 +45068,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="68"/>
+      <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -44431,10 +45162,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="68" t="s">
+      <c r="H19" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="68"/>
+      <c r="I19" s="69"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -44463,10 +45194,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="68" t="s">
+      <c r="H22" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="68"/>
+      <c r="I22" s="69"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -44557,10 +45288,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="68" t="s">
+      <c r="H29" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="68"/>
+      <c r="I29" s="69"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -44584,10 +45315,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="68" t="s">
+      <c r="H32" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="68"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -44675,10 +45406,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="68" t="s">
+      <c r="H39" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="68"/>
+      <c r="I39" s="69"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -44722,10 +45453,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="68" t="s">
+      <c r="H42" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="68"/>
+      <c r="I42" s="69"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -44810,10 +45541,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="68" t="s">
+      <c r="H49" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="68"/>
+      <c r="I49" s="69"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -44857,10 +45588,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="68" t="s">
+      <c r="H52" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="68"/>
+      <c r="I52" s="69"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -44945,10 +45676,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="68" t="s">
+      <c r="H59" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="68"/>
+      <c r="I59" s="69"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -44992,10 +45723,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="68" t="s">
+      <c r="H62" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="68"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -45080,10 +45811,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="68" t="s">
+      <c r="H69" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="68"/>
+      <c r="I69" s="69"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -45127,10 +45858,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="68" t="s">
+      <c r="H72" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="68"/>
+      <c r="I72" s="69"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -45215,10 +45946,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="68" t="s">
+      <c r="H79" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="68"/>
+      <c r="I79" s="69"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -45262,10 +45993,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="68" t="s">
+      <c r="H82" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="68"/>
+      <c r="I82" s="69"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -45350,10 +46081,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="68" t="s">
+      <c r="H89" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="68"/>
+      <c r="I89" s="69"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -45366,12 +46097,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -45384,6 +46109,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -45413,8 +46144,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -45470,8 +46201,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -45487,8 +46218,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -45569,8 +46300,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -45586,8 +46317,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -45666,8 +46397,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -45713,8 +46444,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -47369,8 +48100,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -47424,8 +48155,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>

<commit_message>
Adding solutions for list 8 - 1 to 7, except 6.
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,16 @@
     <sheet name="q7-08" sheetId="10" r:id="rId8"/>
     <sheet name="q7-09" sheetId="8" r:id="rId9"/>
     <sheet name="q7-10" sheetId="11" r:id="rId10"/>
+    <sheet name="q8-01" sheetId="12" r:id="rId11"/>
+    <sheet name="q8-02" sheetId="13" r:id="rId12"/>
+    <sheet name="q8-04" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="93">
   <si>
     <t>l</t>
   </si>
@@ -286,6 +289,27 @@
   </si>
   <si>
     <t>3/4</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>T'</t>
+  </si>
+  <si>
+    <t>T''</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>V - S</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1138,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1232,6 +1256,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,6 +1276,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5833,6 +5866,2363 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector reto 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531575" y="561000"/>
+          <a:ext cx="611550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector reto 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="4"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1351575" y="741000"/>
+          <a:ext cx="0" cy="337275"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Grupo 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="428625" y="381000"/>
+          <a:ext cx="2074500" cy="1057275"/>
+          <a:chOff x="329587" y="276225"/>
+          <a:chExt cx="2074500" cy="1057275"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Conector reto 5"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="9" idx="7"/>
+            <a:endCxn id="7" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="636866" y="456225"/>
+            <a:ext cx="435671" cy="236621"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>t</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>v</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Fluxograma: Conector 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="329587" y="640125"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>s</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="Conector reto 9"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="11" idx="0"/>
+            <a:endCxn id="8" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2224087" y="636225"/>
+            <a:ext cx="0" cy="337275"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Fluxograma: Conector 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Fluxograma: Conector 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>u</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Conector reto 56"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="62" idx="6"/>
+          <a:endCxn id="63" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531575" y="561000"/>
+          <a:ext cx="611550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Conector reto 57"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="62" idx="4"/>
+          <a:endCxn id="67" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1351575" y="741000"/>
+          <a:ext cx="0" cy="337275"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>217125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="59" name="Grupo 58"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3476625" y="381000"/>
+          <a:ext cx="2074500" cy="1057275"/>
+          <a:chOff x="329587" y="276225"/>
+          <a:chExt cx="2074500" cy="1057275"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="60" name="Conector reto 59"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="67" idx="6"/>
+            <a:endCxn id="66" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1432537" y="1153500"/>
+            <a:ext cx="611550" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="61" name="Conector reto 60"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="64" idx="7"/>
+            <a:endCxn id="62" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="636866" y="456225"/>
+            <a:ext cx="435671" cy="236621"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="62" name="Fluxograma: Conector 61"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>t</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="63" name="Fluxograma: Conector 62"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>v</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="64" name="Fluxograma: Conector 63"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="329587" y="640125"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>s</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="66" name="Fluxograma: Conector 65"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="67" name="Fluxograma: Conector 66"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>u</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Conector reto 67"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="72" idx="6"/>
+          <a:endCxn id="73" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531575" y="561000"/>
+          <a:ext cx="611550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>8189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>182311</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Conector reto 68"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="72" idx="4"/>
+          <a:endCxn id="77" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1351575" y="2208464"/>
+          <a:ext cx="0" cy="364622"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="70" name="Grupo 69"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="428625" y="1819275"/>
+          <a:ext cx="2074500" cy="1143000"/>
+          <a:chOff x="329587" y="276225"/>
+          <a:chExt cx="2074500" cy="1057275"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="71" name="Conector reto 70"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="74" idx="7"/>
+            <a:endCxn id="72" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="636866" y="456225"/>
+            <a:ext cx="435671" cy="236621"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="72" name="Fluxograma: Conector 71"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>t</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="73" name="Fluxograma: Conector 72"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>v</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="74" name="Fluxograma: Conector 73"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="329587" y="640125"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>s</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="Conector reto 74"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="76" idx="0"/>
+            <a:endCxn id="73" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="2224087" y="636225"/>
+            <a:ext cx="0" cy="337275"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="76" name="Fluxograma: Conector 75"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>x</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="77" name="Fluxograma: Conector 76"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>u</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>186406</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>186406</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Conector reto 78"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="76" idx="2"/>
+          <a:endCxn id="77" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1531575" y="2767681"/>
+          <a:ext cx="611550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector reto 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531575" y="561000"/>
+          <a:ext cx="602025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>162900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>115275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector reto 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="6"/>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="788625" y="924900"/>
+          <a:ext cx="382950" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217125</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Grupo 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="428625" y="152401"/>
+          <a:ext cx="2074500" cy="1704974"/>
+          <a:chOff x="329587" y="47626"/>
+          <a:chExt cx="2074500" cy="1704974"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Conector reto 4"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="12" idx="6"/>
+            <a:endCxn id="11" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1432537" y="1153500"/>
+            <a:ext cx="611550" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:prstDash val="solid"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Conector reto 5"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="9" idx="6"/>
+            <a:endCxn id="7" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="689587" y="456225"/>
+            <a:ext cx="382950" cy="363900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst>
+            <a:glow rad="63500">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="25000"/>
+                <a:alpha val="40000"/>
+              </a:schemeClr>
+            </a:glow>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>s</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2034562" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>r</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Fluxograma: Conector 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="329587" y="640125"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>t</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="Conector reto 9"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="1653562" y="47626"/>
+            <a:ext cx="0" cy="1704974"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:prstDash val="dash"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Fluxograma: Conector 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>v</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Fluxograma: Conector 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>u</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -41719,6 +44109,568 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>316804</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector reto 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="11" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1307404" y="1142025"/>
+          <a:ext cx="454721" cy="636671"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>189525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>62246</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector reto 4"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="6"/>
+          <a:endCxn id="10" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2122125" y="1142025"/>
+          <a:ext cx="454721" cy="636671"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector reto 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="4"/>
+          <a:endCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1942125" y="550500"/>
+          <a:ext cx="0" cy="411525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="190500"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>a</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Fluxograma: Conector 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="962025"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>b</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector reto 12"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="2"/>
+          <a:endCxn id="11" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1360125" y="1905975"/>
+          <a:ext cx="1164000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Fluxograma: Conector 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="1725975"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>c</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Fluxograma: Conector 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000125" y="1725975"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>d</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -42045,7 +44997,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="65">
+      <c r="B3" s="67">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -42086,7 +45038,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="66"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -42123,7 +45075,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="66"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -42158,7 +45110,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="66"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -42191,7 +45143,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="67"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -42222,7 +45174,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="65">
+      <c r="B8" s="67">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -42253,7 +45205,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="66"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -42271,7 +45223,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="66"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -42292,7 +45244,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="66"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -42328,7 +45280,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="66"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -42367,7 +45319,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -42404,7 +45356,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="66"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -42439,7 +45391,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="67"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -42472,7 +45424,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="65">
+      <c r="B16" s="67">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -42505,7 +45457,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -42534,7 +45486,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="66"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -42552,7 +45504,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="66"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -42570,7 +45522,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="66"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -42588,7 +45540,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="66"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -42606,7 +45558,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="66"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -42624,7 +45576,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="66"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -42642,7 +45594,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="67"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -42660,7 +45612,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="65">
+      <c r="B25" s="67">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -42680,7 +45632,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="66"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -42698,7 +45650,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="66"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -42716,7 +45668,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="66"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -42734,7 +45686,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="66"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -42752,7 +45704,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="66"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -42770,7 +45722,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="66"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -42788,7 +45740,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="67"/>
+      <c r="B32" s="69"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -42806,7 +45758,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="65">
+      <c r="B33" s="67">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -42826,7 +45778,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="66"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -42844,7 +45796,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="66"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -42862,7 +45814,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="66"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -42880,7 +45832,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="67"/>
+      <c r="B37" s="69"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -42914,7 +45866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -42987,6 +45939,326 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="66"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="57"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="66"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="38"/>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="53"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="38"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="57"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="66">
+        <v>3</v>
+      </c>
+      <c r="G8" s="61">
+        <v>3</v>
+      </c>
+      <c r="L8" s="53"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="38"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="57"/>
+      <c r="H10" s="58"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E11" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="66"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="38"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="23" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="66"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="66"/>
+      <c r="J4" s="66"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="G5" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" s="66"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="66"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="66"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="66"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="66"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G13" s="66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="66"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="66"/>
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="25" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="66"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E3" s="38">
+        <v>3</v>
+      </c>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66">
+        <v>1</v>
+      </c>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="52"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="66">
+        <v>2</v>
+      </c>
+      <c r="E7" s="72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="72"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="66"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -43154,8 +46426,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -43227,8 +46499,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -43245,8 +46517,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -43321,8 +46593,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -43345,8 +46617,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -43421,8 +46693,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -43445,8 +46717,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -43518,8 +46790,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -43542,8 +46814,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -43615,8 +46887,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="68"/>
-      <c r="I49" s="68"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="70"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -43639,8 +46911,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -43712,8 +46984,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="68"/>
-      <c r="I59" s="68"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -43773,10 +47045,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="69"/>
+      <c r="I2" s="71"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -43861,10 +47133,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="69" t="s">
+      <c r="H9" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="71"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -43882,10 +47154,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="69" t="s">
+      <c r="H12" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="69"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -43976,10 +47248,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="69" t="s">
+      <c r="H19" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="69"/>
+      <c r="I19" s="71"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -44003,10 +47275,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="69"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -44097,10 +47369,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="69" t="s">
+      <c r="H29" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="69"/>
+      <c r="I29" s="71"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -44124,10 +47396,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="69" t="s">
+      <c r="H32" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="69"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -44215,10 +47487,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="69" t="s">
+      <c r="H39" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="69"/>
+      <c r="I39" s="71"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -44262,10 +47534,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="69" t="s">
+      <c r="H42" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="69"/>
+      <c r="I42" s="71"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -44350,10 +47622,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="69" t="s">
+      <c r="H49" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="69"/>
+      <c r="I49" s="71"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -44397,10 +47669,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="69" t="s">
+      <c r="H52" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="69"/>
+      <c r="I52" s="71"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -44485,10 +47757,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="69" t="s">
+      <c r="H59" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="69"/>
+      <c r="I59" s="71"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -44532,10 +47804,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="69" t="s">
+      <c r="H62" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="69"/>
+      <c r="I62" s="71"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -44620,10 +47892,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="69" t="s">
+      <c r="H69" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="69"/>
+      <c r="I69" s="71"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -44667,10 +47939,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="69" t="s">
+      <c r="H72" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="69"/>
+      <c r="I72" s="71"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -44755,10 +48027,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="69" t="s">
+      <c r="H79" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="69"/>
+      <c r="I79" s="71"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -44802,10 +48074,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="69" t="s">
+      <c r="H82" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="69"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -44890,10 +48162,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="69" t="s">
+      <c r="H89" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="69"/>
+      <c r="I89" s="71"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -44906,12 +48178,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -44924,6 +48190,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44959,10 +48231,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="69"/>
+      <c r="I2" s="71"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -45047,10 +48319,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="69" t="s">
+      <c r="H9" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="71"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -45068,10 +48340,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="69" t="s">
+      <c r="H12" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="69"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -45162,10 +48434,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="69" t="s">
+      <c r="H19" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="69"/>
+      <c r="I19" s="71"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -45194,10 +48466,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="69"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -45288,10 +48560,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="69" t="s">
+      <c r="H29" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="69"/>
+      <c r="I29" s="71"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -45315,10 +48587,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="69" t="s">
+      <c r="H32" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="69"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -45406,10 +48678,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="69" t="s">
+      <c r="H39" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="69"/>
+      <c r="I39" s="71"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -45453,10 +48725,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="69" t="s">
+      <c r="H42" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="69"/>
+      <c r="I42" s="71"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -45541,10 +48813,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="69" t="s">
+      <c r="H49" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="69"/>
+      <c r="I49" s="71"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -45588,10 +48860,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="69" t="s">
+      <c r="H52" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="69"/>
+      <c r="I52" s="71"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -45676,10 +48948,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="69" t="s">
+      <c r="H59" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="69"/>
+      <c r="I59" s="71"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -45723,10 +48995,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="69" t="s">
+      <c r="H62" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="69"/>
+      <c r="I62" s="71"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -45811,10 +49083,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="69" t="s">
+      <c r="H69" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="69"/>
+      <c r="I69" s="71"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -45858,10 +49130,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="69" t="s">
+      <c r="H72" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="69"/>
+      <c r="I72" s="71"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -45946,10 +49218,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="69" t="s">
+      <c r="H79" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="69"/>
+      <c r="I79" s="71"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -45993,10 +49265,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="69" t="s">
+      <c r="H82" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="69"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -46081,10 +49353,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="69" t="s">
+      <c r="H89" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="69"/>
+      <c r="I89" s="71"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -46097,6 +49369,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -46109,12 +49387,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -46144,8 +49416,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -46201,8 +49473,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -46218,8 +49490,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -46300,8 +49572,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -46317,8 +49589,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -46397,8 +49669,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -46444,8 +49716,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -48100,8 +51372,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -48155,8 +51427,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>

<commit_message>
Adding solution for CLRS 23.1-4 and fixing minor issues.
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="q8-01" sheetId="12" r:id="rId11"/>
     <sheet name="q8-02" sheetId="13" r:id="rId12"/>
     <sheet name="q8-04" sheetId="14" r:id="rId13"/>
+    <sheet name="q8-05-1" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1138,7 +1139,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1262,6 +1263,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8223,6 +8233,427 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>316804</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>126304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62246</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector reto 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="9" idx="7"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1307404" y="1269304"/>
+          <a:ext cx="507442" cy="509392"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>316804</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>126304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>62246</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64196</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector reto 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="5"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2069404" y="1269304"/>
+          <a:ext cx="507442" cy="509392"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Fluxograma: Conector 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1762125" y="962025"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>a</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector reto 6"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="9" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1360125" y="1905975"/>
+          <a:ext cx="1164000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="1725975"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>c</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>369525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Fluxograma: Conector 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000125" y="1725975"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>b</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -44997,7 +45428,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="67">
+      <c r="B3" s="70">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -45038,7 +45469,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="68"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -45075,7 +45506,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="68"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -45110,7 +45541,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="68"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -45143,7 +45574,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -45174,7 +45605,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="67">
+      <c r="B8" s="70">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -45205,7 +45636,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -45223,7 +45654,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -45244,7 +45675,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -45280,7 +45711,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -45319,7 +45750,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -45356,7 +45787,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -45391,7 +45822,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -45424,7 +45855,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="67">
+      <c r="B16" s="70">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -45457,7 +45888,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -45486,7 +45917,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="68"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -45504,7 +45935,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="68"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -45522,7 +45953,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="68"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -45540,7 +45971,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="68"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -45558,7 +45989,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="68"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -45576,7 +46007,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="68"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -45594,7 +46025,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="69"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -45612,7 +46043,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="67">
+      <c r="B25" s="70">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -45632,7 +46063,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="68"/>
+      <c r="B26" s="71"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -45650,7 +46081,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="68"/>
+      <c r="B27" s="71"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -45668,7 +46099,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="68"/>
+      <c r="B28" s="71"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -45686,7 +46117,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="68"/>
+      <c r="B29" s="71"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -45704,7 +46135,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
+      <c r="B30" s="71"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -45722,7 +46153,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="68"/>
+      <c r="B31" s="71"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -45740,7 +46171,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="69"/>
+      <c r="B32" s="72"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -45758,7 +46189,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="67">
+      <c r="B33" s="70">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -45778,7 +46209,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
+      <c r="B34" s="71"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -45796,7 +46227,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -45814,7 +46245,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
+      <c r="B36" s="71"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -45832,7 +46263,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="69"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -45967,8 +46398,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57"/>
@@ -46023,8 +46454,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="66"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
       <c r="L12" s="38"/>
       <c r="M12" s="65"/>
       <c r="N12" s="39"/>
@@ -46066,8 +46497,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="66"/>
@@ -46095,8 +46526,8 @@
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
       <c r="J9" s="66"/>
       <c r="K9" s="1"/>
       <c r="L9" s="66"/>
@@ -46147,7 +46578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -46165,8 +46596,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E3" s="38">
@@ -46224,12 +46655,12 @@
       <c r="C7" s="66">
         <v>2</v>
       </c>
-      <c r="E7" s="72">
+      <c r="E7" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="72"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="66"/>
@@ -46238,8 +46669,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
       <c r="K9" s="38"/>
       <c r="L9" s="65"/>
       <c r="M9" s="39"/>
@@ -46258,6 +46689,105 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H9:I9"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C1" s="68"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="57"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="68"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="69"/>
+      <c r="E4" s="1"/>
+      <c r="L4" s="53"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="69"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="57"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D8" s="61">
+        <v>3</v>
+      </c>
+      <c r="F8" s="69">
+        <v>3</v>
+      </c>
+      <c r="L8" s="53"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="69"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="57"/>
+      <c r="H10" s="58"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E11" s="68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="68"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="69"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -46426,8 +46956,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -46499,8 +47029,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -46517,8 +47047,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -46593,8 +47123,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -46617,8 +47147,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -46693,8 +47223,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="73"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -46717,8 +47247,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="73"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -46790,8 +47320,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="70"/>
-      <c r="I39" s="70"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -46814,8 +47344,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -46887,8 +47417,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="70"/>
-      <c r="I49" s="70"/>
+      <c r="H49" s="73"/>
+      <c r="I49" s="73"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -46911,8 +47441,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="70"/>
-      <c r="I52" s="70"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -46984,8 +47514,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="70"/>
-      <c r="I59" s="70"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -47045,10 +47575,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="71"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -47133,10 +47663,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="74"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -47154,10 +47684,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="71"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -47248,10 +47778,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="71" t="s">
+      <c r="H19" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="71"/>
+      <c r="I19" s="74"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -47275,10 +47805,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="71" t="s">
+      <c r="H22" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="74"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -47369,10 +47899,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="71"/>
+      <c r="I29" s="74"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -47396,10 +47926,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="71" t="s">
+      <c r="H32" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="71"/>
+      <c r="I32" s="74"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -47487,10 +48017,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="71" t="s">
+      <c r="H39" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="71"/>
+      <c r="I39" s="74"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -47534,10 +48064,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="71"/>
+      <c r="I42" s="74"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -47622,10 +48152,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="71" t="s">
+      <c r="H49" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="71"/>
+      <c r="I49" s="74"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -47669,10 +48199,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="71"/>
+      <c r="I52" s="74"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -47757,10 +48287,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="71" t="s">
+      <c r="H59" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="71"/>
+      <c r="I59" s="74"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -47804,10 +48334,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="71" t="s">
+      <c r="H62" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="71"/>
+      <c r="I62" s="74"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -47892,10 +48422,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="71" t="s">
+      <c r="H69" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="71"/>
+      <c r="I69" s="74"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -47939,10 +48469,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="71" t="s">
+      <c r="H72" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="71"/>
+      <c r="I72" s="74"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -48027,10 +48557,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="71" t="s">
+      <c r="H79" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="71"/>
+      <c r="I79" s="74"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -48074,10 +48604,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="71" t="s">
+      <c r="H82" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="71"/>
+      <c r="I82" s="74"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -48162,10 +48692,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="71" t="s">
+      <c r="H89" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="71"/>
+      <c r="I89" s="74"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -48178,6 +48708,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -48190,12 +48726,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -48231,10 +48761,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="71"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -48319,10 +48849,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="74"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -48340,10 +48870,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="71"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -48434,10 +48964,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="71" t="s">
+      <c r="H19" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="71"/>
+      <c r="I19" s="74"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -48466,10 +48996,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="71" t="s">
+      <c r="H22" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="74"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -48560,10 +49090,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="71" t="s">
+      <c r="H29" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="71"/>
+      <c r="I29" s="74"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -48587,10 +49117,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="71" t="s">
+      <c r="H32" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="71"/>
+      <c r="I32" s="74"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -48678,10 +49208,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="71" t="s">
+      <c r="H39" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="71"/>
+      <c r="I39" s="74"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -48725,10 +49255,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="71" t="s">
+      <c r="H42" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="71"/>
+      <c r="I42" s="74"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -48813,10 +49343,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="71" t="s">
+      <c r="H49" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="71"/>
+      <c r="I49" s="74"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -48860,10 +49390,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="71" t="s">
+      <c r="H52" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="71"/>
+      <c r="I52" s="74"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -48948,10 +49478,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="71" t="s">
+      <c r="H59" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="71"/>
+      <c r="I59" s="74"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -48995,10 +49525,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="71" t="s">
+      <c r="H62" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="71"/>
+      <c r="I62" s="74"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -49083,10 +49613,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="71" t="s">
+      <c r="H69" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="71"/>
+      <c r="I69" s="74"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -49130,10 +49660,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="71" t="s">
+      <c r="H72" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="71"/>
+      <c r="I72" s="74"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -49218,10 +49748,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="71" t="s">
+      <c r="H79" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="71"/>
+      <c r="I79" s="74"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -49265,10 +49795,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="71" t="s">
+      <c r="H82" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="71"/>
+      <c r="I82" s="74"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -49353,10 +49883,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="71" t="s">
+      <c r="H89" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="71"/>
+      <c r="I89" s="74"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -49369,12 +49899,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -49387,6 +49911,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49416,8 +49946,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -49473,8 +50003,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -49490,8 +50020,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -49572,8 +50102,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -49589,8 +50119,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -49669,8 +50199,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -49716,8 +50246,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -51372,8 +51902,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -51427,8 +51957,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>

<commit_message>
Adding anser for q8-18
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
     <sheet name="q8-02" sheetId="13" r:id="rId12"/>
     <sheet name="q8-04" sheetId="14" r:id="rId13"/>
     <sheet name="q8-05-1" sheetId="15" r:id="rId14"/>
+    <sheet name="q8-18" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="93">
   <si>
     <t>l</t>
   </si>
@@ -1139,7 +1140,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1272,6 +1273,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8654,6 +8664,521 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>37125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>37125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Conector reto 14"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="4"/>
+          <a:endCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2323125" y="741000"/>
+          <a:ext cx="0" cy="337275"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector reto 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531575" y="561000"/>
+          <a:ext cx="611550" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>217125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Grupo 3"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1171575" y="381000"/>
+          <a:ext cx="1331550" cy="1057275"/>
+          <a:chOff x="1072537" y="276225"/>
+          <a:chExt cx="1331550" cy="1057275"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="Conector reto 4"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="12" idx="6"/>
+            <a:endCxn id="11" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1432537" y="1153500"/>
+            <a:ext cx="611550" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:prstDash val="solid"/>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="none"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Conector reto 5"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="7" idx="4"/>
+            <a:endCxn id="12" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1252537" y="636225"/>
+            <a:ext cx="0" cy="337275"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+          <a:effectLst>
+            <a:glow rad="63500">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="25000"/>
+                <a:alpha val="40000"/>
+              </a:schemeClr>
+            </a:glow>
+          </a:effectLst>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>0</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="Fluxograma: Conector 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1072537" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>1</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Fluxograma: Conector 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="973500"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>0</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2044087" y="276225"/>
+            <a:ext cx="360000" cy="360000"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartConnector">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>2</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -45428,7 +45953,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="70">
+      <c r="B3" s="73">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -45469,7 +45994,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="71"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -45506,7 +46031,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="71"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -45541,7 +46066,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="71"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -45574,7 +46099,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -45605,7 +46130,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="70">
+      <c r="B8" s="73">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -45636,7 +46161,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="71"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -45654,7 +46179,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="71"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -45675,7 +46200,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="71"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -45711,7 +46236,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="71"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -45750,7 +46275,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="71"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -45787,7 +46312,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="71"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -45822,7 +46347,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="72"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -45855,7 +46380,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="70">
+      <c r="B16" s="73">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -45888,7 +46413,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="71"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -45917,7 +46442,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="71"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -45935,7 +46460,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="71"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -45953,7 +46478,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="71"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -45971,7 +46496,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="71"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -45989,7 +46514,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -46007,7 +46532,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="71"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -46025,7 +46550,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="72"/>
+      <c r="B24" s="75"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -46043,7 +46568,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="70">
+      <c r="B25" s="73">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -46063,7 +46588,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="71"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -46081,7 +46606,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="71"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -46099,7 +46624,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="71"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -46117,7 +46642,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="71"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -46135,7 +46660,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="71"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -46153,7 +46678,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="71"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -46171,7 +46696,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="72"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -46189,7 +46714,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="70">
+      <c r="B33" s="73">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -46209,7 +46734,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="71"/>
+      <c r="B34" s="74"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -46227,7 +46752,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="71"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -46245,7 +46770,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="71"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -46263,7 +46788,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="72"/>
+      <c r="B37" s="75"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -46398,8 +46923,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57"/>
@@ -46454,8 +46979,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="66"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
       <c r="L12" s="38"/>
       <c r="M12" s="65"/>
       <c r="N12" s="39"/>
@@ -46497,8 +47022,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="66"/>
@@ -46526,8 +47051,8 @@
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
       <c r="J9" s="66"/>
       <c r="K9" s="1"/>
       <c r="L9" s="66"/>
@@ -46596,8 +47121,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E3" s="38">
@@ -46655,12 +47180,12 @@
       <c r="C7" s="66">
         <v>2</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="78">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="75"/>
+      <c r="E8" s="78"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="66"/>
@@ -46669,8 +47194,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
       <c r="K9" s="38"/>
       <c r="L9" s="65"/>
       <c r="M9" s="39"/>
@@ -46700,7 +47225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -46718,8 +47243,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="69"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57"/>
@@ -46772,8 +47297,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="68"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
       <c r="L12" s="69"/>
       <c r="M12" s="67"/>
       <c r="N12" s="39"/>
@@ -46788,6 +47313,134 @@
   <mergeCells count="2">
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="25" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="71"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E3" s="72">
+        <v>2</v>
+      </c>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="72"/>
+      <c r="D5" s="61">
+        <v>1</v>
+      </c>
+      <c r="G5" s="71">
+        <v>-2</v>
+      </c>
+      <c r="K5" s="49"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="52"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="71"/>
+      <c r="E7" s="78">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="78"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="71"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="72"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -46956,8 +47609,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -47029,8 +47682,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -47047,8 +47700,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -47123,8 +47776,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -47147,8 +47800,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -47223,8 +47876,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -47247,8 +47900,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -47320,8 +47973,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -47344,8 +47997,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -47417,8 +48070,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="73"/>
-      <c r="I49" s="73"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -47441,8 +48094,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="73"/>
-      <c r="I52" s="73"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -47514,8 +48167,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="73"/>
-      <c r="I59" s="73"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -47575,10 +48228,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="74"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -47663,10 +48316,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="74" t="s">
+      <c r="H9" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="74"/>
+      <c r="I9" s="77"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -47684,10 +48337,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -47778,10 +48431,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="74" t="s">
+      <c r="H19" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="74"/>
+      <c r="I19" s="77"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -47805,10 +48458,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="74" t="s">
+      <c r="H22" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="74"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -47899,10 +48552,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="74" t="s">
+      <c r="H29" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="74"/>
+      <c r="I29" s="77"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -47926,10 +48579,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="74" t="s">
+      <c r="H32" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="74"/>
+      <c r="I32" s="77"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -48017,10 +48670,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="74" t="s">
+      <c r="H39" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="74"/>
+      <c r="I39" s="77"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -48064,10 +48717,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="74" t="s">
+      <c r="H42" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="74"/>
+      <c r="I42" s="77"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -48152,10 +48805,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="74" t="s">
+      <c r="H49" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="74"/>
+      <c r="I49" s="77"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -48199,10 +48852,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="74" t="s">
+      <c r="H52" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="74"/>
+      <c r="I52" s="77"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -48287,10 +48940,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="74" t="s">
+      <c r="H59" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="74"/>
+      <c r="I59" s="77"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -48334,10 +48987,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="74" t="s">
+      <c r="H62" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="74"/>
+      <c r="I62" s="77"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -48422,10 +49075,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="74" t="s">
+      <c r="H69" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="74"/>
+      <c r="I69" s="77"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -48469,10 +49122,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="74" t="s">
+      <c r="H72" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="74"/>
+      <c r="I72" s="77"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -48557,10 +49210,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="74" t="s">
+      <c r="H79" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="74"/>
+      <c r="I79" s="77"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -48604,10 +49257,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="74" t="s">
+      <c r="H82" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="74"/>
+      <c r="I82" s="77"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -48692,10 +49345,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="74" t="s">
+      <c r="H89" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="74"/>
+      <c r="I89" s="77"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -48708,12 +49361,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -48726,6 +49373,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -48761,10 +49414,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="74"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -48849,10 +49502,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="74" t="s">
+      <c r="H9" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="74"/>
+      <c r="I9" s="77"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -48870,10 +49523,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -48964,10 +49617,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="74" t="s">
+      <c r="H19" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="74"/>
+      <c r="I19" s="77"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -48996,10 +49649,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="74" t="s">
+      <c r="H22" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="74"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -49090,10 +49743,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="74" t="s">
+      <c r="H29" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="74"/>
+      <c r="I29" s="77"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -49117,10 +49770,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="74" t="s">
+      <c r="H32" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="74"/>
+      <c r="I32" s="77"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -49208,10 +49861,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="74" t="s">
+      <c r="H39" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="74"/>
+      <c r="I39" s="77"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -49255,10 +49908,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="74" t="s">
+      <c r="H42" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="74"/>
+      <c r="I42" s="77"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -49343,10 +49996,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="74" t="s">
+      <c r="H49" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="74"/>
+      <c r="I49" s="77"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -49390,10 +50043,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="74" t="s">
+      <c r="H52" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="74"/>
+      <c r="I52" s="77"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -49478,10 +50131,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="74" t="s">
+      <c r="H59" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="74"/>
+      <c r="I59" s="77"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -49525,10 +50178,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="74" t="s">
+      <c r="H62" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="74"/>
+      <c r="I62" s="77"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -49613,10 +50266,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="74" t="s">
+      <c r="H69" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="74"/>
+      <c r="I69" s="77"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -49660,10 +50313,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="74" t="s">
+      <c r="H72" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="74"/>
+      <c r="I72" s="77"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -49748,10 +50401,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="74" t="s">
+      <c r="H79" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="74"/>
+      <c r="I79" s="77"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -49795,10 +50448,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="74" t="s">
+      <c r="H82" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="74"/>
+      <c r="I82" s="77"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -49883,10 +50536,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="74" t="s">
+      <c r="H89" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="74"/>
+      <c r="I89" s="77"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -49899,6 +50552,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -49911,12 +50570,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49946,8 +50599,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -50003,8 +50656,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -50020,8 +50673,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -50102,8 +50755,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -50119,8 +50772,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -50199,8 +50852,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -50246,8 +50899,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -51902,8 +52555,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -51957,8 +52610,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>

<commit_message>
Adding solution for q8-10
</commit_message>
<xml_diff>
--- a/algorithms/mac-5711-tex/files/debugging.xlsx
+++ b/algorithms/mac-5711-tex/files/debugging.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="2" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="q6-01" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,15 @@
     <sheet name="q8-02" sheetId="13" r:id="rId12"/>
     <sheet name="q8-04" sheetId="14" r:id="rId13"/>
     <sheet name="q8-05-1" sheetId="15" r:id="rId14"/>
-    <sheet name="q8-18" sheetId="16" r:id="rId15"/>
+    <sheet name="q8-10" sheetId="17" r:id="rId15"/>
+    <sheet name="q8-18" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="95">
   <si>
     <t>l</t>
   </si>
@@ -312,6 +313,12 @@
   </si>
   <si>
     <t>V - S</t>
+  </si>
+  <si>
+    <t>V - Q</t>
+  </si>
+  <si>
+    <t>Conjunto</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1147,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1282,6 +1289,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1299,6 +1315,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -8670,6 +8692,1872 @@
 </file>
 
 <file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector reto 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="8" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2550750" y="1227750"/>
+          <a:ext cx="1211625" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector reto 2"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="6"/>
+          <a:endCxn id="12" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="788625" y="924900"/>
+          <a:ext cx="430575" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector reto 4"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="6"/>
+          <a:endCxn id="11" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2550750" y="2115525"/>
+          <a:ext cx="1211625" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector reto 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="788625" y="465750"/>
+          <a:ext cx="430575" cy="459150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3762375" y="1047750"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝒘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝟑</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="Fluxograma: Conector 7"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3762375" y="1047750"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝒘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝟑</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>173400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Fluxograma: Conector 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="428625" y="744900"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>0</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Fluxograma: Conector 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762375" y="1935525"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>∞</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Fluxograma: Conector 11"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1219200" y="1173525"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝒘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝟐</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Fluxograma: Conector 11"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1219200" y="1173525"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝒘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝟐</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>36150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Fluxograma: Conector 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="1047751"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>∞</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>36150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Fluxograma: Conector 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="1935526"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>∞</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>121876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Fluxograma: Conector 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952625" y="714376"/>
+          <a:ext cx="360000" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>∞</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>256200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>256200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector reto 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="4"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1399200" y="645750"/>
+          <a:ext cx="0" cy="527775"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="63500">
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2479</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69155</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100346</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>83246</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector reto 18"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="7"/>
+          <a:endCxn id="15" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1526479" y="1021655"/>
+          <a:ext cx="478867" cy="204591"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>26625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>21529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>176546</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>132376</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector reto 22"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="6"/>
+          <a:endCxn id="8" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3284175" y="1355029"/>
+          <a:ext cx="530921" cy="301347"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74250</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1219200" y="285750"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1050" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1050" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒘</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1050" b="1" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝟏</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1050" b="1" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝒘</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1050" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Fluxograma: Conector 6"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1219200" y="285750"/>
+              <a:ext cx="360000" cy="360000"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartConnector">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+              <a:prstTxWarp prst="textNoShape">
+                <a:avLst/>
+              </a:prstTxWarp>
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="r" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1050" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>𝒘</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1050" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1050" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>𝟏 𝒘</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1050" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>318633</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>112712</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>77982</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Arco 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="4908302">
+          <a:off x="958864" y="-47416"/>
+          <a:ext cx="1390167" cy="2670629"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 15078944"/>
+            <a:gd name="adj2" fmla="val 3575244"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>84751</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector reto 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="6"/>
+          <a:endCxn id="13" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4122375" y="1227750"/>
+          <a:ext cx="640125" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>160950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>160950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector reto 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="0"/>
+          <a:endCxn id="13" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4942500" y="1407751"/>
+          <a:ext cx="0" cy="527775"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>303825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>74250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>303825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector reto 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="0"/>
+          <a:endCxn id="8" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3942375" y="1407750"/>
+          <a:ext cx="0" cy="527775"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20026</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Conector reto 36"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="6"/>
+          <a:endCxn id="14" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4122375" y="2115525"/>
+          <a:ext cx="640125" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="none"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -45953,7 +47841,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="73">
+      <c r="B3" s="76">
         <v>2</v>
       </c>
       <c r="C3" s="13">
@@ -45994,7 +47882,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="74"/>
+      <c r="B4" s="77"/>
       <c r="C4" s="21">
         <v>2</v>
       </c>
@@ -46031,7 +47919,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="74"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="21">
         <v>3</v>
       </c>
@@ -46066,7 +47954,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="74"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="21">
         <v>4</v>
       </c>
@@ -46099,7 +47987,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="75"/>
+      <c r="B7" s="78"/>
       <c r="C7" s="5">
         <v>5</v>
       </c>
@@ -46130,7 +48018,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="73">
+      <c r="B8" s="76">
         <v>3</v>
       </c>
       <c r="C8" s="6">
@@ -46161,7 +48049,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="74"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="14">
         <v>1</v>
       </c>
@@ -46179,7 +48067,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="74"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="16">
         <v>2</v>
       </c>
@@ -46200,7 +48088,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="74"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>
@@ -46236,7 +48124,7 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
@@ -46275,7 +48163,7 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="14">
         <v>3</v>
       </c>
@@ -46312,7 +48200,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="74"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="5">
         <v>4</v>
       </c>
@@ -46347,7 +48235,7 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="75"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="5">
         <v>4</v>
       </c>
@@ -46380,7 +48268,7 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="73">
+      <c r="B16" s="76">
         <v>4</v>
       </c>
       <c r="C16" s="6">
@@ -46413,7 +48301,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="74"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="5">
         <v>1</v>
       </c>
@@ -46442,7 +48330,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="14">
         <v>1</v>
       </c>
@@ -46460,7 +48348,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="74"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="16">
         <v>2</v>
       </c>
@@ -46478,7 +48366,7 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="74"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="5">
         <v>2</v>
       </c>
@@ -46496,7 +48384,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="74"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="14">
         <v>2</v>
       </c>
@@ -46514,7 +48402,7 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="74"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="5">
         <v>3</v>
       </c>
@@ -46532,7 +48420,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="74"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -46550,7 +48438,7 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="75"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -46568,7 +48456,7 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="73">
+      <c r="B25" s="76">
         <v>5</v>
       </c>
       <c r="C25" s="6">
@@ -46588,7 +48476,7 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="74"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="5">
         <v>1</v>
       </c>
@@ -46606,7 +48494,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="74"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="5">
         <v>1</v>
       </c>
@@ -46624,7 +48512,7 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="74"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="14">
         <v>1</v>
       </c>
@@ -46642,7 +48530,7 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="74"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="5">
         <v>2</v>
       </c>
@@ -46660,7 +48548,7 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="74"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="5">
         <v>2</v>
       </c>
@@ -46678,7 +48566,7 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="74"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
@@ -46696,7 +48584,7 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="75"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="5">
         <v>2</v>
       </c>
@@ -46714,7 +48602,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="73">
+      <c r="B33" s="76">
         <v>6</v>
       </c>
       <c r="C33" s="6">
@@ -46734,7 +48622,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="74"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="5">
         <v>1</v>
       </c>
@@ -46752,7 +48640,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="74"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -46770,7 +48658,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="74"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -46788,7 +48676,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="75"/>
+      <c r="B37" s="78"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -46923,8 +48811,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57"/>
@@ -46979,8 +48867,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="66"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
       <c r="L12" s="38"/>
       <c r="M12" s="65"/>
       <c r="N12" s="39"/>
@@ -47022,8 +48910,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="66"/>
@@ -47051,8 +48939,8 @@
       </c>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
       <c r="J9" s="66"/>
       <c r="K9" s="1"/>
       <c r="L9" s="66"/>
@@ -47121,8 +49009,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E3" s="38">
@@ -47180,12 +49068,12 @@
       <c r="C7" s="66">
         <v>2</v>
       </c>
-      <c r="E7" s="78">
+      <c r="E7" s="81">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="78"/>
+      <c r="E8" s="81"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="66"/>
@@ -47194,8 +49082,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="66"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
       <c r="K9" s="38"/>
       <c r="L9" s="65"/>
       <c r="M9" s="39"/>
@@ -47243,8 +49131,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="69"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57"/>
@@ -47297,8 +49185,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="68"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
       <c r="L12" s="69"/>
       <c r="M12" s="67"/>
       <c r="N12" s="39"/>
@@ -47322,9 +49210,132 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:T14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F7" s="75"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="74"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="75"/>
+      <c r="B9" s="75"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L10" s="52"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D11" s="74"/>
+      <c r="F11" s="81"/>
+    </row>
+    <row r="12" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="81"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="74"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="39"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D14" s="75"/>
+      <c r="G14" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="I13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
@@ -47346,8 +49357,8 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E3" s="72">
@@ -47407,12 +49418,12 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="71"/>
-      <c r="E7" s="78">
+      <c r="E7" s="81">
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="78"/>
+      <c r="E8" s="81"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
@@ -47425,8 +49436,8 @@
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
       <c r="M9" s="39"/>
@@ -47586,7 +49597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
@@ -47609,8 +49620,8 @@
       <c r="F2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -47682,8 +49693,8 @@
       <c r="F9" s="43">
         <v>6</v>
       </c>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -47700,8 +49711,8 @@
       <c r="F12" s="38">
         <v>3</v>
       </c>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -47776,8 +49787,8 @@
       <c r="F19" s="43">
         <v>6</v>
       </c>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -47800,8 +49811,8 @@
       <c r="F22" s="38">
         <v>3</v>
       </c>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -47876,8 +49887,8 @@
       <c r="F29" s="43">
         <v>6</v>
       </c>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -47900,8 +49911,8 @@
       <c r="F32" s="38">
         <v>3</v>
       </c>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -47973,8 +49984,8 @@
       <c r="F39" s="43">
         <v>6</v>
       </c>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -47997,8 +50008,8 @@
       <c r="F42" s="38">
         <v>3</v>
       </c>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
+      <c r="H42" s="79"/>
+      <c r="I42" s="79"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -48070,8 +50081,8 @@
       <c r="F49" s="43">
         <v>6</v>
       </c>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="79"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -48094,8 +50105,8 @@
       <c r="F52" s="38">
         <v>3</v>
       </c>
-      <c r="H52" s="76"/>
-      <c r="I52" s="76"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -48167,8 +50178,8 @@
       <c r="F59" s="43">
         <v>6</v>
       </c>
-      <c r="H59" s="76"/>
-      <c r="I59" s="76"/>
+      <c r="H59" s="79"/>
+      <c r="I59" s="79"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -48228,10 +50239,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="77"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -48316,10 +50327,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="77"/>
+      <c r="I9" s="80"/>
       <c r="K9" s="38"/>
       <c r="L9" s="36"/>
       <c r="M9" s="39"/>
@@ -48337,10 +50348,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="77"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -48431,10 +50442,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="77" t="s">
+      <c r="H19" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="77"/>
+      <c r="I19" s="80"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -48458,10 +50469,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="77" t="s">
+      <c r="H22" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="77"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -48552,10 +50563,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="77" t="s">
+      <c r="H29" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="77"/>
+      <c r="I29" s="80"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -48579,10 +50590,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="77" t="s">
+      <c r="H32" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="77"/>
+      <c r="I32" s="80"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -48670,10 +50681,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="77" t="s">
+      <c r="H39" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="77"/>
+      <c r="I39" s="80"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -48717,10 +50728,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="77" t="s">
+      <c r="H42" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="77"/>
+      <c r="I42" s="80"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -48805,10 +50816,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="77" t="s">
+      <c r="H49" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="77"/>
+      <c r="I49" s="80"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -48852,10 +50863,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="77" t="s">
+      <c r="H52" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="77"/>
+      <c r="I52" s="80"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -48940,10 +50951,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="77" t="s">
+      <c r="H59" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="77"/>
+      <c r="I59" s="80"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -48987,10 +50998,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="77" t="s">
+      <c r="H62" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="77"/>
+      <c r="I62" s="80"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -49075,10 +51086,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="77" t="s">
+      <c r="H69" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="77"/>
+      <c r="I69" s="80"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -49122,10 +51133,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="77" t="s">
+      <c r="H72" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="77"/>
+      <c r="I72" s="80"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -49210,10 +51221,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="77" t="s">
+      <c r="H79" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="77"/>
+      <c r="I79" s="80"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -49257,10 +51268,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="77" t="s">
+      <c r="H82" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="77"/>
+      <c r="I82" s="80"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -49345,10 +51356,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="77" t="s">
+      <c r="H89" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="77"/>
+      <c r="I89" s="80"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -49361,6 +51372,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -49373,12 +51390,6 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49414,10 +51425,10 @@
         <v>20</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="77"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="34" t="s">
@@ -49502,10 +51513,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="77"/>
+      <c r="I9" s="80"/>
       <c r="K9" s="38"/>
       <c r="L9" s="37"/>
       <c r="M9" s="39"/>
@@ -49523,10 +51534,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="77"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34" t="s">
@@ -49617,10 +51628,10 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="77" t="s">
+      <c r="H19" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="77"/>
+      <c r="I19" s="80"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
@@ -49649,10 +51660,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="77" t="s">
+      <c r="H22" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="77"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K23" s="34" t="s">
@@ -49743,10 +51754,10 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="77" t="s">
+      <c r="H29" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="77"/>
+      <c r="I29" s="80"/>
       <c r="K29" s="38" t="s">
         <v>14</v>
       </c>
@@ -49770,10 +51781,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="77" t="s">
+      <c r="H32" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="77"/>
+      <c r="I32" s="80"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K33" s="34" t="s">
@@ -49861,10 +51872,10 @@
         <v>25</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="77" t="s">
+      <c r="H39" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="77"/>
+      <c r="I39" s="80"/>
       <c r="K39" s="38" t="s">
         <v>14</v>
       </c>
@@ -49908,10 +51919,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="77" t="s">
+      <c r="H42" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="77"/>
+      <c r="I42" s="80"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K43" s="34" t="s">
@@ -49996,10 +52007,10 @@
         <v>25</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="77" t="s">
+      <c r="H49" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I49" s="77"/>
+      <c r="I49" s="80"/>
       <c r="K49" s="38" t="s">
         <v>14</v>
       </c>
@@ -50043,10 +52054,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="77" t="s">
+      <c r="H52" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="77"/>
+      <c r="I52" s="80"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K53" s="34" t="s">
@@ -50131,10 +52142,10 @@
         <v>25</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="77" t="s">
+      <c r="H59" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="77"/>
+      <c r="I59" s="80"/>
       <c r="K59" s="38" t="s">
         <v>14</v>
       </c>
@@ -50178,10 +52189,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="77" t="s">
+      <c r="H62" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I62" s="77"/>
+      <c r="I62" s="80"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K63" s="34" t="s">
@@ -50266,10 +52277,10 @@
         <v>25</v>
       </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="77" t="s">
+      <c r="H69" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="77"/>
+      <c r="I69" s="80"/>
       <c r="K69" s="38" t="s">
         <v>14</v>
       </c>
@@ -50313,10 +52324,10 @@
         <v>20</v>
       </c>
       <c r="G72" s="1"/>
-      <c r="H72" s="77" t="s">
+      <c r="H72" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="77"/>
+      <c r="I72" s="80"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K73" s="34" t="s">
@@ -50401,10 +52412,10 @@
         <v>25</v>
       </c>
       <c r="G79" s="1"/>
-      <c r="H79" s="77" t="s">
+      <c r="H79" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="77"/>
+      <c r="I79" s="80"/>
       <c r="K79" s="38" t="s">
         <v>14</v>
       </c>
@@ -50448,10 +52459,10 @@
         <v>20</v>
       </c>
       <c r="G82" s="1"/>
-      <c r="H82" s="77" t="s">
+      <c r="H82" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="77"/>
+      <c r="I82" s="80"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K83" s="34" t="s">
@@ -50536,10 +52547,10 @@
         <v>25</v>
       </c>
       <c r="G89" s="1"/>
-      <c r="H89" s="77" t="s">
+      <c r="H89" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I89" s="77"/>
+      <c r="I89" s="80"/>
       <c r="K89" s="38" t="s">
         <v>14</v>
       </c>
@@ -50552,12 +52563,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H89:I89"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H39:I39"/>
@@ -50570,6 +52575,12 @@
     <mergeCell ref="H72:I72"/>
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H22:I22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -50599,8 +52610,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="38"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K3" s="49"/>
@@ -50656,8 +52667,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="46"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
       <c r="K9" s="38"/>
       <c r="L9" s="45"/>
       <c r="M9" s="39"/>
@@ -50673,8 +52684,8 @@
         <v>15</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="34"/>
@@ -50755,8 +52766,8 @@
         <v>25</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
       <c r="K19" s="38"/>
       <c r="L19" s="45"/>
       <c r="M19" s="39"/>
@@ -50772,8 +52783,8 @@
         <v>15</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
       <c r="K22" s="34"/>
       <c r="L22" s="33" t="s">
         <v>6</v>
@@ -50852,8 +52863,8 @@
         <v>25</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
       <c r="K29" s="38"/>
       <c r="L29" s="45"/>
       <c r="M29" s="39"/>
@@ -50899,8 +52910,8 @@
       <c r="E1" s="1"/>
       <c r="F1" s="38"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="57"/>
@@ -52555,8 +54566,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="38"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D2" s="57" t="s">
@@ -52610,8 +54621,8 @@
       <c r="F12" s="1"/>
       <c r="G12" s="48"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
       <c r="L12" s="38"/>
       <c r="M12" s="47"/>
       <c r="N12" s="39"/>

</xml_diff>